<commit_message>
GiovanniPC: Domingo 14 de Febrero de 2016
</commit_message>
<xml_diff>
--- a/docs/MaestrosSagrado.xlsx
+++ b/docs/MaestrosSagrado.xlsx
@@ -190,8 +190,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -219,8 +227,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +527,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -529,16 +538,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -740,6 +749,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>